<commit_message>
update references in security-assessment-template.xlsx
</commit_message>
<xml_diff>
--- a/security-assessment-template.xlsx
+++ b/security-assessment-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6fac00b57f9d0812/work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="214" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99C48337-48F9-498E-A18E-C71F0461AEDF}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F2C6FAE-58C1-4864-BD0B-4541635BBD7A}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="89">
   <si>
     <t>Id</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>link</t>
+  </si>
+  <si>
+    <t>https://github.com/gnairooze/security/blob/main/website-api-db-security.md</t>
+  </si>
+  <si>
+    <t>website api db security</t>
   </si>
 </sst>
 </file>
@@ -309,7 +315,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,6 +343,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -355,10 +369,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -378,28 +393,16 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="165" formatCode="[$-409]dd\-mmm\-yy;@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -622,7 +625,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{DE18EB0F-4D64-40D0-B9AB-B54FBEEDB253}" name="Id"/>
     <tableColumn id="2" xr3:uid="{A69AAC3A-19A7-4B3C-942A-6597EB6EBD26}" name="title" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{07CD26CF-09B0-442C-983B-3023536AF7D1}" name="link" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{07CD26CF-09B0-442C-983B-3023536AF7D1}" name="link" dataDxfId="0" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -964,14 +967,14 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="3" max="3" width="71.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1034,8 +1037,12 @@
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="D7" s="8"/>
     </row>
     <row r="9" spans="1:4" ht="31.5">
@@ -1077,10 +1084,13 @@
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{3864C1B2-55EE-44BE-BB10-39784161189D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>